<commit_message>
Aggiornato Test 450 e relativi File
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ELCO0000000/EL_CO_/Fenix-cce/v3_19_05/report-checklist.xlsx
+++ b/GATEWAY/A1#111ELCO0000000/EL_CO_/Fenix-cce/v3_19_05/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FSE VALIDAZIONE\it-fse-accreditamento\GATEWAY\A1#111ELCO0000000\EL_CO_\Fenix-cce\v3_19_05\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\FSE VALIDAZIONE\it-fse-accreditamento\GATEWAY\A1#111ELCO0000000\EL_CO_\Fenix-cce\v3_19_05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A91A46-EB20-43A2-AE90-F9CED49FA58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D14EC3A-DB2F-47EC-A58B-AA42E65C4ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1744,15 +1744,6 @@
     <t>Il campo action_id non è corretto</t>
   </si>
   <si>
-    <t>2025-07-24T12:17:06.854Z</t>
-  </si>
-  <si>
-    <t>f99ee81f1a839f4b85a2fa93aecaf462</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.70.4.4.33cffdc05a08eb8bd8bfc7b167e2f7609f9dabfb5eb43e8eddcc4200c444a07f.0e5f516a40^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2025-07-24T12:30:05.864Z</t>
   </si>
   <si>
@@ -1847,6 +1838,15 @@
   </si>
   <si>
     <t>FSE warning: ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element '{"urn:hl7-org:v3":languageCode}'. One of '{"urn:hl7-org:v3":confidentialityCode}' is expected.</t>
+  </si>
+  <si>
+    <t>2025-08-21T14:44:44.074Z</t>
+  </si>
+  <si>
+    <t>0c79b96bf2cc2a182ff35d984c04bdb4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.70.4.4.33cffdc05a08eb8bd8bfc7b167e2f7609f9dabfb5eb43e8eddcc4200c444a07f.ad98c7e238^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3916,10 +3916,10 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="S1" activeCellId="10" sqref="L169 F1:F1048576 G1:G1048576 H1:H1048576 I1:I1048576 M1:M1048576 N1:N1048576 P1:P1048576 Q1:Q1048576 R1:R1048576 S1:S1048576"/>
+      <selection pane="bottomRight" activeCell="I169" sqref="I169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4300,10 +4300,10 @@
         <v>45497</v>
       </c>
       <c r="G12" s="37" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="H12" s="37" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="I12" s="42" t="s">
         <v>443</v>
@@ -4620,10 +4620,10 @@
         <v>45497</v>
       </c>
       <c r="G20" s="37" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="H20" s="37" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="I20" s="42" t="s">
         <v>443</v>
@@ -5529,13 +5529,13 @@
         <v>45497</v>
       </c>
       <c r="G43" s="37" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="H43" s="37" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="I43" s="42" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="J43" s="38" t="s">
         <v>64</v>
@@ -5549,7 +5549,7 @@
         <v>64</v>
       </c>
       <c r="O43" s="38" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="P43" s="38" t="s">
         <v>64</v>
@@ -5590,13 +5590,13 @@
         <v>45497</v>
       </c>
       <c r="G44" s="37" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="H44" s="37" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="I44" s="42" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="J44" s="38" t="s">
         <v>64</v>
@@ -5610,7 +5610,7 @@
         <v>64</v>
       </c>
       <c r="O44" s="38" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="P44" s="38" t="s">
         <v>64</v>
@@ -5651,13 +5651,13 @@
         <v>45497</v>
       </c>
       <c r="G45" s="37" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H45" s="37" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="I45" s="42" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="J45" s="38" t="s">
         <v>64</v>
@@ -5671,7 +5671,7 @@
         <v>64</v>
       </c>
       <c r="O45" s="38" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="P45" s="38" t="s">
         <v>64</v>
@@ -5712,13 +5712,13 @@
         <v>45497</v>
       </c>
       <c r="G46" s="37" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="H46" s="37" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="I46" s="42" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="J46" s="38" t="s">
         <v>64</v>
@@ -5732,7 +5732,7 @@
         <v>64</v>
       </c>
       <c r="O46" s="38" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="P46" s="38" t="s">
         <v>64</v>
@@ -5773,13 +5773,13 @@
         <v>45497</v>
       </c>
       <c r="G47" s="37" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H47" s="37" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="I47" s="42" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="J47" s="38" t="s">
         <v>64</v>
@@ -5793,7 +5793,7 @@
         <v>64</v>
       </c>
       <c r="O47" s="38" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="P47" s="38" t="s">
         <v>64</v>
@@ -5834,13 +5834,13 @@
         <v>45497</v>
       </c>
       <c r="G48" s="37" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="H48" s="37" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="I48" s="42" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="J48" s="38" t="s">
         <v>64</v>
@@ -5854,7 +5854,7 @@
         <v>64</v>
       </c>
       <c r="O48" s="38" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="P48" s="38" t="s">
         <v>64</v>
@@ -10311,16 +10311,16 @@
         <v>373</v>
       </c>
       <c r="F168" s="37">
-        <v>45497</v>
+        <v>45890</v>
       </c>
       <c r="G168" s="37" t="s">
-        <v>447</v>
+        <v>479</v>
       </c>
       <c r="H168" s="37" t="s">
-        <v>448</v>
+        <v>480</v>
       </c>
       <c r="I168" s="42" t="s">
-        <v>449</v>
+        <v>481</v>
       </c>
       <c r="J168" s="38" t="s">
         <v>64</v>
@@ -10920,13 +10920,13 @@
         <v>45497</v>
       </c>
       <c r="G184" s="35" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="H184" s="38" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="I184" s="38" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="J184" s="38" t="s">
         <v>64</v>
@@ -10940,7 +10940,7 @@
         <v>64</v>
       </c>
       <c r="O184" s="38" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="P184" s="38" t="s">
         <v>64</v>
@@ -17564,15 +17564,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17834,27 +17831,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17879,9 +17870,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>